<commit_message>
Updated to loop and fit constant of proportionality
Jon,

I agree with your comments about the lambda not being necessary. I
updated the code to loop through each value of n multiple times. This
better displayed the fit when solving for the constant of
proportionality.

Also, I updated the code to automatically do the fit.
</commit_message>
<xml_diff>
--- a/src/timing.xlsx
+++ b/src/timing.xlsx
@@ -13,17 +13,17 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">timings!$H$4</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">timings!$J$4</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>|Samples</t>
   </si>
@@ -45,11 +45,26 @@
   <si>
     <t>diff</t>
   </si>
+  <si>
+    <t>alpha_py</t>
+  </si>
+  <si>
+    <t>py_sq_diff</t>
+  </si>
+  <si>
+    <t>py_diff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0000000_);_(* \(#,##0.0000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -484,7 +499,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -527,11 +542,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -559,6 +579,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -671,37 +692,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.01114946173326E-3</c:v>
+                  <c:v>1.3543341402329E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.96226056663626E-3</c:v>
+                  <c:v>1.8484192823389499E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8594542043751301E-3</c:v>
+                  <c:v>2.90305052737149E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.77620340015281E-3</c:v>
+                  <c:v>4.7499333015788299E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.82173991387173E-3</c:v>
+                  <c:v>0.113618909665893</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3067177532340001E-3</c:v>
+                  <c:v>0.22646733034505701</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.44751777111336E-3</c:v>
+                  <c:v>0.45075309850832901</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4514037398607903E-3</c:v>
+                  <c:v>0.94426833578010605</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.4974738409490501E-3</c:v>
+                  <c:v>2.3601549917657101</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.20157729543838E-2</c:v>
+                  <c:v>5.4147141605986198</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.23955837962646E-2</c:v>
+                  <c:v>11.794370234205701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -710,7 +731,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>timings!$D$1</c:f>
@@ -732,37 +753,98 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.7874936544081787E-5</c:v>
+                  <c:v>5.0664056942890346E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0218607224184021E-5</c:v>
+                  <c:v>1.1399412812150327E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.9374682720408936E-5</c:v>
+                  <c:v>2.5332028471445174E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9662430198489966E-4</c:v>
+                  <c:v>5.573046263717938E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2899847705796289E-4</c:v>
+                  <c:v>0.12159373666293682</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.2949670029225293E-4</c:v>
+                  <c:v>0.2634530961030298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0019928929371602E-3</c:v>
+                  <c:v>0.56743743776037192</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2899847705796289E-3</c:v>
+                  <c:v>1.2159373666293682</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.151967510569875E-3</c:v>
+                  <c:v>2.5939997154759857</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9447930959960984E-2</c:v>
+                  <c:v>5.51224939538647</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.1183853797564438E-2</c:v>
+                  <c:v>11.672998719641935</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>timings!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>alpha_py</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>timings!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.0000000_);_(* \(#,##0.0000000\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.06250428416E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1390634639359999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.53125214208E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5687547125760004E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12150010281984</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26325022277631999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56700047982592006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2150010281984001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.59200219348992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5080046611660798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.664009870704639</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -779,88 +861,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="310114944"/>
-        <c:axId val="312680832"/>
-      </c:lineChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>timings!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>n*log_2(n)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>timings!$C$2:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4608</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10240</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22528</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49152</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>106496</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>229376</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>491520</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1048576</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2228224</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4718592</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="327867008"/>
-        <c:axId val="327864704"/>
+        <c:axId val="301647360"/>
+        <c:axId val="301648896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="310114944"/>
+        <c:axId val="301647360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="312680832"/>
+        <c:crossAx val="301648896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -878,7 +883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312680832"/>
+        <c:axId val="301648896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,41 +894,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="310114944"/>
+        <c:crossAx val="301647360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:valAx>
-        <c:axId val="327864704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="327867008"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="327867008"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="327864704"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -1264,18 +1238,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1291,238 +1270,349 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>256</v>
       </c>
       <c r="B2">
-        <v>2.01114946173326E-3</v>
+        <v>1.3543341402329E-2</v>
       </c>
       <c r="C2">
         <f>A2*LOG(A2,2)</f>
         <v>2048</v>
       </c>
       <c r="D2">
-        <f>C2*$I$2</f>
-        <v>1.7874936544081787E-5</v>
+        <f t="shared" ref="D2:D12" si="0">C2*$K$2</f>
+        <v>5.0664056942890346E-3</v>
       </c>
       <c r="E2">
         <f>(B2-D2)^2</f>
-        <v>3.9731433327681447E-6</v>
-      </c>
-      <c r="H2" t="s">
+        <v>7.185843899824302E-5</v>
+      </c>
+      <c r="F2" s="2">
+        <f t="shared" ref="F2:F12" si="1">C2*$K$5</f>
+        <v>5.06250428416E-3</v>
+      </c>
+      <c r="G2">
+        <f>(B2-F2)^2</f>
+        <v>7.1924598224913072E-5</v>
+      </c>
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="I2">
-        <v>8.7279963594149351E-9</v>
+      <c r="K2" s="4">
+        <v>2.4738309054145677E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>512</v>
       </c>
       <c r="B3">
-        <v>1.96226056663626E-3</v>
+        <v>1.8484192823389499E-2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C12" si="0">A3*LOG(A3,2)</f>
+        <f t="shared" ref="C3:C12" si="2">A3*LOG(A3,2)</f>
         <v>4608</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D12" si="1">C3*$I$2</f>
-        <v>4.0218607224184021E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.1399412812150327E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E12" si="2">(B3-D3)^2</f>
-        <v>3.6942452937406126E-6</v>
-      </c>
-      <c r="H3" t="s">
+        <f t="shared" ref="E3:E12" si="3">(B3-D3)^2</f>
+        <v>5.0194107807654115E-5</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1390634639359999E-2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="4">(B3-F3)^2</f>
+        <v>5.0318567710211898E-5</v>
+      </c>
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <f>SUM(E:E)</f>
-        <v>4.3263905420972635E-4</v>
+        <v>0.1679818462356652</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1024</v>
       </c>
       <c r="B4">
-        <v>1.8594542043751301E-3</v>
+        <v>2.90305052737149E-2</v>
       </c>
       <c r="C4">
+        <f t="shared" si="2"/>
+        <v>10240</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
-        <v>10240</v>
-      </c>
-      <c r="D4">
+        <v>2.5332028471445174E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>1.3678730656927294E-5</v>
+      </c>
+      <c r="F4" s="2">
         <f t="shared" si="1"/>
-        <v>8.9374682720408936E-5</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="2"/>
-        <v>3.133181512981406E-6</v>
+        <v>2.53125214208E-2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="4"/>
+        <v>1.382340393053592E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2048</v>
       </c>
       <c r="B5">
-        <v>1.77620340015281E-3</v>
+        <v>4.7499333015788299E-2</v>
       </c>
       <c r="C5">
+        <f t="shared" si="2"/>
+        <v>22528</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
-        <v>22528</v>
-      </c>
-      <c r="D5">
+        <v>5.573046263717938E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>6.7751494844141679E-5</v>
+      </c>
+      <c r="F5" s="2">
         <f t="shared" si="1"/>
-        <v>1.9662430198489966E-4</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>2.4950701273689491E-6</v>
+        <v>5.5687547125760004E-2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>6.7046850310739715E-5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2.47192592E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4096</v>
       </c>
       <c r="B6">
-        <v>1.82173991387173E-3</v>
+        <v>0.113618909665893</v>
       </c>
       <c r="C6">
+        <f t="shared" si="2"/>
+        <v>49152</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>49152</v>
-      </c>
-      <c r="D6">
+        <v>0.12159373666293682</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>6.3597865632779061E-5</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
-        <v>4.2899847705796289E-4</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>1.9397287098180764E-6</v>
+        <v>0.12150010281984</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>6.2113205529821101E-5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="3">
+        <f>SUM(G2:G12)</f>
+        <v>0.16787791902417479</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8192</v>
       </c>
       <c r="B7">
-        <v>2.3067177532340001E-3</v>
+        <v>0.22646733034505701</v>
       </c>
       <c r="C7">
+        <f t="shared" si="2"/>
+        <v>106496</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>106496</v>
-      </c>
-      <c r="D7">
+        <v>0.2634530961030298</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>1.3679468687036332E-3</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>9.2949670029225293E-4</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>1.8967378286659748E-6</v>
+        <v>0.26325022277631999</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>1.3529811756098635E-3</v>
+      </c>
+      <c r="K7" t="b">
+        <f>K6&lt;K3</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16384</v>
       </c>
       <c r="B8">
-        <v>2.44751777111336E-3</v>
+        <v>0.45075309850832901</v>
       </c>
       <c r="C8">
+        <f t="shared" si="2"/>
+        <v>229376</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>229376</v>
-      </c>
-      <c r="D8">
+        <v>0.56743743776037192</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>1.3615235026685843E-2</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
-        <v>2.0019928929371602E-3</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
-        <v>1.9849241707391769E-7</v>
+        <v>0.56700047982592006</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>1.3513453663197415E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>32768</v>
       </c>
       <c r="B9">
-        <v>4.4514037398607903E-3</v>
+        <v>0.94426833578010605</v>
       </c>
       <c r="C9">
+        <f t="shared" si="2"/>
+        <v>491520</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>491520</v>
-      </c>
-      <c r="D9">
+        <v>1.2159373666293682</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>7.3804062322577371E-2</v>
+      </c>
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>4.2899847705796289E-3</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>2.6056083643792525E-8</v>
+        <v>1.2150010281984001</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>7.329619074405859E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>65536</v>
       </c>
       <c r="B10">
-        <v>6.4974738409490501E-3</v>
+        <v>2.3601549917657101</v>
       </c>
       <c r="C10">
+        <f t="shared" si="2"/>
+        <v>1048576</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>1048576</v>
-      </c>
-      <c r="D10">
+        <v>2.5939997154759857</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>5.4683354807135154E-2</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>9.151967510569875E-3</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="2"/>
-        <v>7.0463366420570328E-6</v>
+        <v>2.59200219348992</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>5.3753124947346485E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>131072</v>
       </c>
       <c r="B11">
-        <v>1.20157729543838E-2</v>
+        <v>5.4147141605986198</v>
       </c>
       <c r="C11">
+        <f t="shared" si="2"/>
+        <v>2228224</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
-        <v>2228224</v>
-      </c>
-      <c r="D11">
+        <v>5.51224939538647</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>9.5131220251210638E-3</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>1.9447930959960984E-2</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="2"/>
-        <v>5.5236972619865023E-5</v>
+        <v>5.5080046611660798</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>8.7031174961272589E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>262144</v>
       </c>
       <c r="B12">
-        <v>2.23955837962646E-2</v>
+        <v>11.794370234205701</v>
       </c>
       <c r="C12">
+        <f t="shared" si="2"/>
+        <v>4718592</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="0"/>
-        <v>4718592</v>
-      </c>
-      <c r="D12">
+        <v>11.672998719641935</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>1.4731044547502393E-2</v>
+      </c>
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>4.1183853797564438E-2</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="2"/>
-        <v>3.5299908964174341E-4</v>
+        <v>11.664009870704639</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>1.6993824372128947E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>